<commit_message>
vault backup: 2022-04-18 23:26:53
</commit_message>
<xml_diff>
--- a/实习指导文件/质量监督表.xlsx
+++ b/实习指导文件/质量监督表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>质量监督表</t>
   </si>
@@ -24,30 +24,54 @@
     <t>承办律师</t>
   </si>
   <si>
+    <t>周平</t>
+  </si>
+  <si>
     <t>委托人</t>
   </si>
   <si>
+    <t>安徽商贸职业技术学院</t>
+  </si>
+  <si>
     <t>联系电话</t>
   </si>
   <si>
     <t>对方当事人</t>
   </si>
   <si>
+    <t>国华工程科技（集团）有限责任公司</t>
+  </si>
+  <si>
     <t>案  由</t>
   </si>
   <si>
+    <t>合同纠纷</t>
+  </si>
+  <si>
     <t>法院案号</t>
   </si>
   <si>
+    <t>（2021）芜仲字第340号</t>
+  </si>
+  <si>
     <t>收案日期</t>
   </si>
   <si>
+    <t>2021.10.21</t>
+  </si>
+  <si>
     <t>结案日期</t>
   </si>
   <si>
+    <t>2022.4.11</t>
+  </si>
+  <si>
     <t>办理结果</t>
   </si>
   <si>
+    <t>裁决被申请人支付附加工作酬金</t>
+  </si>
+  <si>
     <t>监  督  项  目</t>
   </si>
   <si>
@@ -57,13 +81,19 @@
     <t xml:space="preserve"> 1、是否由律师事务所与委托人签订委托代理合同。</t>
   </si>
   <si>
-    <t>是□  否□</t>
+    <t>是☑  否□</t>
   </si>
   <si>
     <t xml:space="preserve"> 2、是否由律师事务所向委托人收取律师代理费并如实开具发票。</t>
   </si>
   <si>
+    <t>是☑   否□</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 3、接受委托后承办律师是否在律师代理费外收取了其它费用、额外报酬或财务。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">是□  否☑ </t>
   </si>
   <si>
     <t xml:space="preserve"> 4、接受委托后承办律师有无泄露当事人商业秘密或者个人隐私的行为。</t>
@@ -98,9 +128,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -126,14 +156,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -141,6 +172,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -148,17 +188,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -170,39 +204,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,55 +234,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,43 +309,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,31 +447,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,19 +465,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,79 +489,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,26 +564,37 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,16 +615,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,7 +633,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,20 +655,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,10 +669,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -651,137 +681,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -797,44 +827,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1188,7 +1215,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1215,184 +1242,201 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" ht="42.75" customHeight="1" spans="1:6">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" ht="61" customHeight="1" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" ht="42.75" customHeight="1" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" ht="42.75" customHeight="1" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" ht="46" customHeight="1" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" ht="37" customHeight="1" spans="1:6">
-      <c r="A7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" ht="37" customHeight="1" spans="1:6">
-      <c r="A8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" ht="42" customHeight="1" spans="1:6">
-      <c r="A9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" ht="36" customHeight="1" spans="1:6">
-      <c r="A10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
+      <c r="A10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" ht="42" customHeight="1" spans="1:6">
-      <c r="A11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" ht="36" customHeight="1" spans="1:6">
-      <c r="A12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" ht="42" customHeight="1" spans="1:6">
-      <c r="A13" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" ht="38" customHeight="1" spans="1:6">
-      <c r="A14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" ht="38" customHeight="1" spans="1:6">
-      <c r="A15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" ht="40" customHeight="1" spans="1:1">
-      <c r="A16" s="18" t="s">
-        <v>22</v>
+      <c r="A16" s="17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="6:6">
       <c r="F21" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2022-10-09 23:42:49
</commit_message>
<xml_diff>
--- a/实习指导文件/质量监督表.xlsx
+++ b/实习指导文件/质量监督表.xlsx
@@ -30,7 +30,7 @@
     <t>委托人</t>
   </si>
   <si>
-    <t>安徽商贸职业技术学院</t>
+    <t>芜湖方不圆工业设计有限公司</t>
   </si>
   <si>
     <t>联系电话</t>
@@ -39,37 +39,37 @@
     <t>对方当事人</t>
   </si>
   <si>
-    <t>国华工程科技（集团）有限责任公司</t>
+    <t>芜湖松鸿金属制品有限公司</t>
   </si>
   <si>
     <t>案  由</t>
   </si>
   <si>
-    <t>合同纠纷</t>
+    <t>财产保全损害责任纠纷</t>
   </si>
   <si>
     <t>法院案号</t>
   </si>
   <si>
-    <t>（2021）芜仲字第340号</t>
+    <t>（2022）皖0291民初1343号</t>
   </si>
   <si>
     <t>收案日期</t>
   </si>
   <si>
-    <t>2021.10.21</t>
+    <t>2022.5.9</t>
   </si>
   <si>
     <t>结案日期</t>
   </si>
   <si>
-    <t>2022.4.11</t>
+    <t>2022.7.18</t>
   </si>
   <si>
     <t>办理结果</t>
   </si>
   <si>
-    <t>裁决被申请人支付附加工作酬金</t>
+    <t>判决驳回原告诉讼请求</t>
   </si>
   <si>
     <t>监  督  项  目</t>
@@ -128,10 +128,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -156,17 +156,76 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,52 +240,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -234,20 +247,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -256,45 +287,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,19 +309,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,37 +399,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,121 +477,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,36 +565,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,17 +594,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,6 +608,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,6 +650,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -669,10 +669,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -681,137 +681,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -850,12 +850,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1214,8 +1208,8 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1317,73 +1311,73 @@
       </c>
     </row>
     <row r="7" ht="37" customHeight="1" spans="1:6">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" ht="37" customHeight="1" spans="1:6">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" ht="42" customHeight="1" spans="1:6">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" ht="36" customHeight="1" spans="1:6">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" ht="42" customHeight="1" spans="1:6">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" ht="36" customHeight="1" spans="1:6">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1425,7 +1419,7 @@
       </c>
     </row>
     <row r="16" ht="40" customHeight="1" spans="1:1">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="15" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vault backup: 2022-10-14 14:55:34
</commit_message>
<xml_diff>
--- a/实习指导文件/质量监督表.xlsx
+++ b/实习指导文件/质量监督表.xlsx
@@ -30,7 +30,7 @@
     <t>委托人</t>
   </si>
   <si>
-    <t>芜湖方不圆工业设计有限公司</t>
+    <t>芜湖众宇环保建材有限公司</t>
   </si>
   <si>
     <t>联系电话</t>
@@ -39,37 +39,37 @@
     <t>对方当事人</t>
   </si>
   <si>
-    <t>芜湖松鸿金属制品有限公司</t>
+    <t>安徽金鹏建设集团股份有限公司</t>
   </si>
   <si>
     <t>案  由</t>
   </si>
   <si>
-    <t>财产保全损害责任纠纷</t>
+    <t>买卖合同纠纷</t>
   </si>
   <si>
     <t>法院案号</t>
   </si>
   <si>
-    <t>（2022）皖0291民初1343号</t>
+    <t>（2022）皖1103民初26号</t>
   </si>
   <si>
     <t>收案日期</t>
   </si>
   <si>
-    <t>2022.5.9</t>
+    <t>2021.11.09</t>
   </si>
   <si>
     <t>结案日期</t>
   </si>
   <si>
-    <t>2022.7.18</t>
+    <t>2022.1.14</t>
   </si>
   <si>
     <t>办理结果</t>
   </si>
   <si>
-    <t>判决驳回原告诉讼请求</t>
+    <t>调解结案</t>
   </si>
   <si>
     <t>监  督  项  目</t>
@@ -1208,8 +1208,8 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
vault backup: 2024-07-01 10:09:41
</commit_message>
<xml_diff>
--- a/实习指导文件/质量监督表.xlsx
+++ b/实习指导文件/质量监督表.xlsx
@@ -4,19 +4,32 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="20752" windowHeight="9555"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>质量监督表</t>
   </si>
@@ -24,13 +37,13 @@
     <t>承办律师</t>
   </si>
   <si>
-    <t>周平</t>
+    <t>徐子介、承涛</t>
   </si>
   <si>
     <t>委托人</t>
   </si>
   <si>
-    <t>芜湖众宇环保建材有限公司</t>
+    <t>张根水</t>
   </si>
   <si>
     <t>联系电话</t>
@@ -39,7 +52,7 @@
     <t>对方当事人</t>
   </si>
   <si>
-    <t>安徽金鹏建设集团股份有限公司</t>
+    <t>江胜、南陵县胜福小麦种植家庭农场、韩芬、南陵汇福农业有限公司</t>
   </si>
   <si>
     <t>案  由</t>
@@ -51,25 +64,25 @@
     <t>法院案号</t>
   </si>
   <si>
-    <t>（2022）皖1103民初26号</t>
+    <t>（2024）皖0223民初1734号</t>
   </si>
   <si>
     <t>收案日期</t>
   </si>
   <si>
-    <t>2021.11.09</t>
+    <t>2024.4.9</t>
   </si>
   <si>
     <t>结案日期</t>
   </si>
   <si>
-    <t>2022.1.14</t>
+    <t>2024.4.15</t>
   </si>
   <si>
     <t>办理结果</t>
   </si>
   <si>
-    <t>调解结案</t>
+    <t>部分支持原告诉讼请求</t>
   </si>
   <si>
     <t>监  督  项  目</t>
@@ -118,15 +131,12 @@
   </si>
   <si>
     <t>安徽承义（芜湖）律师事务所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  年   月   日</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -156,55 +166,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -249,6 +223,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -294,7 +283,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,49 +319,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,121 +457,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,21 +575,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -608,6 +603,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -666,152 +676,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -833,24 +843,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -859,56 +872,59 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1206,19 +1222,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.1111111111111" customWidth="1"/>
-    <col min="2" max="2" width="18.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="11.8796296296296" customWidth="1"/>
-    <col min="4" max="4" width="13.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="13.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="14.1150442477876" customWidth="1"/>
+    <col min="2" max="2" width="20.2477876106195" customWidth="1"/>
+    <col min="3" max="3" width="11.8761061946903" customWidth="1"/>
+    <col min="4" max="4" width="13.3362831858407" customWidth="1"/>
+    <col min="5" max="5" width="13.7787610619469" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1254,10 +1270,10 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1266,11 +1282,11 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" ht="42.75" customHeight="1" spans="1:6">
+    <row r="4" ht="50" customHeight="1" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1290,13 +1306,13 @@
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" ht="46" customHeight="1" spans="1:6">
       <c r="A6" s="3" t="s">
@@ -1311,126 +1327,126 @@
       </c>
     </row>
     <row r="7" ht="37" customHeight="1" spans="1:6">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" ht="37" customHeight="1" spans="1:6">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" ht="42" customHeight="1" spans="1:6">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" ht="36" customHeight="1" spans="1:6">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" ht="42" customHeight="1" spans="1:6">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" ht="36" customHeight="1" spans="1:6">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" ht="42" customHeight="1" spans="1:6">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" ht="38" customHeight="1" spans="1:6">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" ht="38" customHeight="1" spans="1:6">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" ht="40" customHeight="1" spans="1:1">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="5:5">
-      <c r="E19" s="1" t="s">
+    <row r="17" spans="5:5">
+      <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="6:6">
-      <c r="F21" s="1" t="s">
-        <v>34</v>
+    <row r="18" spans="6:6">
+      <c r="F18" s="17">
+        <v>45405</v>
       </c>
     </row>
   </sheetData>
@@ -1448,7 +1464,7 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.786805555555556" right="0.511805555555556" top="0.747916666666667" bottom="0.747916666666667" header="0.314583333333333" footer="0.314583333333333"/>
@@ -1466,7 +1482,7 @@
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1482,7 +1498,7 @@
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>